<commit_message>
Neue Datenbank für MySQL-Workbench! Implementierungen folgen!
</commit_message>
<xml_diff>
--- a/Datenbank/Relationales Modell.xlsx
+++ b/Datenbank/Relationales Modell.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\do-it-later\Datenbank\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Softwareprojekte\do-it-later\Datenbank\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC4D9D-0B69-454C-8B70-08D308254008}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,76 +25,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>USER</t>
   </si>
   <si>
-    <t>UserID</t>
-  </si>
-  <si>
     <t>Int</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Varchar(50)</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>GROUP</t>
-  </si>
-  <si>
-    <t>GroupID</t>
-  </si>
-  <si>
-    <t>GroupName</t>
-  </si>
-  <si>
     <t>Varchar(20)</t>
   </si>
   <si>
-    <t>fk_GroupAdmin</t>
-  </si>
-  <si>
     <t>USER_IN_GROUP</t>
   </si>
   <si>
-    <t>fk_UserID</t>
-  </si>
-  <si>
-    <t>fk_GroupID</t>
-  </si>
-  <si>
     <t>TASK</t>
   </si>
   <si>
-    <t>TaskID</t>
-  </si>
-  <si>
     <t>AUTO_INC</t>
   </si>
   <si>
-    <t>Titel</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Beschreibung</t>
-  </si>
-  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>BOARD</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>FK TO user.name</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>group_id</t>
+  </si>
+  <si>
+    <t>FK TO board.id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>bearbeiter</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>Varchar(12)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +114,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,11 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -172,7 +195,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -484,16 +507,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -503,130 +527,142 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
+      <c r="A16" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>